<commit_message>
final changes before ordering
</commit_message>
<xml_diff>
--- a/bom/backplane_bom.xlsx
+++ b/bom/backplane_bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Internal Research and Development\RD17 Spacecraft Subsystems and Components\Backplane\KiCad\CubeSat_Backplane\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Github\backplane\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="CubeSat_Backplane" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
   <si>
     <t>Item</t>
   </si>
@@ -99,12 +99,6 @@
     <t>TLH-030-0.50-G-D-A</t>
   </si>
   <si>
-    <t>M3</t>
-  </si>
-  <si>
-    <t>CubeSat_Backplane:M3_PTH_PAD</t>
-  </si>
-  <si>
     <t>BC857AW,115</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>J300, J301</t>
   </si>
   <si>
-    <t>MH100, MH101, MH102, MH103, MH104, MH105</t>
-  </si>
-  <si>
     <t>Q600, Q601, Q602</t>
   </si>
   <si>
@@ -208,6 +199,30 @@
   </si>
   <si>
     <t>RMCF0402FT10K0</t>
+  </si>
+  <si>
+    <t>J101</t>
+  </si>
+  <si>
+    <t>DF13-4P-1.25V(76)</t>
+  </si>
+  <si>
+    <t>CubeSat_Backplane:DF13-4P-1.25(75)</t>
+  </si>
+  <si>
+    <t>BURN_WIRES</t>
+  </si>
+  <si>
+    <t>X+ SOLAR PANEL</t>
+  </si>
+  <si>
+    <t>X- SOLAR PANEL</t>
+  </si>
+  <si>
+    <t>Y+ SOLAR PANEL</t>
+  </si>
+  <si>
+    <t>DNI</t>
   </si>
 </sst>
 </file>
@@ -708,9 +723,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1035,7 +1051,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1079,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1076,7 +1092,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1096,7 +1112,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -1116,7 +1132,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -1158,6 +1174,9 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="E6" t="s">
         <v>17</v>
       </c>
@@ -1175,6 +1194,9 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="E7" t="s">
         <v>17</v>
       </c>
@@ -1192,6 +1214,9 @@
       <c r="C8" t="s">
         <v>20</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E8" t="s">
         <v>17</v>
       </c>
@@ -1207,7 +1232,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -1224,36 +1249,39 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1264,16 +1292,16 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1284,16 +1312,16 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
         <v>29</v>
-      </c>
-      <c r="F13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1304,16 +1332,16 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1324,16 +1352,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1344,19 +1372,19 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1364,19 +1392,19 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1384,19 +1412,19 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1404,19 +1432,22 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
         <v>42</v>
       </c>
-      <c r="E19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1424,16 +1455,16 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>